<commit_message>
V2 MCU firmware Alfa release
</commit_message>
<xml_diff>
--- a/docs/Рассчет тепловыделения.xlsx
+++ b/docs/Рассчет тепловыделения.xlsx
@@ -148,9 +148,6 @@
     <t>LTC6752HS5</t>
   </si>
   <si>
-    <t>SN74LV1T34</t>
-  </si>
-  <si>
     <t>Unreg. voltage (VDC) CoilV3</t>
   </si>
   <si>
@@ -188,6 +185,9 @@
   </si>
   <si>
     <t>2xLTC2057HV</t>
+  </si>
+  <si>
+    <t>2xSN74LV1T34</t>
   </si>
 </sst>
 </file>
@@ -610,7 +610,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -627,9 +627,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -651,9 +648,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -686,6 +680,23 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -722,26 +733,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1026,7 +1032,7 @@
   <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1037,10 +1043,11 @@
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="10.7265625" customWidth="1"/>
     <col min="8" max="8" width="13.08984375" customWidth="1"/>
-    <col min="9" max="9" width="14.90625" customWidth="1"/>
+    <col min="9" max="9" width="12.6328125" customWidth="1"/>
     <col min="10" max="10" width="7.7265625" customWidth="1"/>
     <col min="11" max="11" width="7.6328125" customWidth="1"/>
-    <col min="12" max="13" width="11.54296875" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" customWidth="1"/>
+    <col min="13" max="13" width="13.1796875" customWidth="1"/>
     <col min="14" max="14" width="11.08984375" customWidth="1"/>
     <col min="15" max="15" width="15.1796875" customWidth="1"/>
     <col min="16" max="16" width="9.54296875" customWidth="1"/>
@@ -1052,150 +1059,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="3" customFormat="1" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="55" t="s">
-        <v>52</v>
+      <c r="A1" s="39" t="s">
+        <v>51</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" s="15" t="s">
+      <c r="S1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="S1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="W1" s="16" t="s">
+      <c r="W1" s="15" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="55"/>
+      <c r="A2" s="39"/>
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31">
+      <c r="C2" s="28"/>
+      <c r="D2" s="29">
         <v>50</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32">
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30">
         <v>0.1</v>
       </c>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32">
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30">
         <v>15</v>
       </c>
-      <c r="L2" s="32">
+      <c r="L2" s="30">
         <v>4.5</v>
       </c>
-      <c r="M2" s="32">
+      <c r="M2" s="30">
         <f>1.5*2</f>
         <v>3</v>
       </c>
-      <c r="N2" s="32">
+      <c r="N2" s="30">
         <v>6</v>
       </c>
-      <c r="O2" s="33">
+      <c r="O2" s="31">
         <v>11.2</v>
       </c>
-      <c r="P2" s="45">
+      <c r="P2" s="50">
         <f>SUM(C2:O2)+SUM(C3:O3)</f>
         <v>269.8</v>
       </c>
-      <c r="Q2" s="39">
+      <c r="Q2" s="44">
         <f>P2*5/1000</f>
         <v>1.349</v>
       </c>
-      <c r="R2" s="47">
+      <c r="R2" s="52">
         <f>'Рассчет трансформатора'!G6</f>
         <v>9.9329999999999998</v>
       </c>
-      <c r="S2" s="49">
+      <c r="S2" s="54">
         <v>6800</v>
       </c>
-      <c r="T2" s="39">
+      <c r="T2" s="44">
         <f>((P2/1000)*0.02)/(S2/1000000)</f>
         <v>0.79352941176470593</v>
       </c>
-      <c r="U2" s="39">
+      <c r="U2" s="44">
         <f>(T2/10000)*1000000</f>
         <v>79.352941176470594</v>
       </c>
-      <c r="V2" s="41">
+      <c r="V2" s="46">
         <f>R2-T2/2-5</f>
         <v>4.5362352941176471</v>
       </c>
-      <c r="W2" s="43">
+      <c r="W2" s="48">
         <f>(R2-5)*P2/1000</f>
         <v>1.3309233999999999</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A3" s="55"/>
+      <c r="A3" s="39"/>
       <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="34">
+      <c r="C3" s="32">
         <v>148</v>
       </c>
-      <c r="D3" s="35"/>
+      <c r="D3" s="33"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2">
@@ -1211,23 +1218,23 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="46"/>
-      <c r="Q3" s="40"/>
-      <c r="R3" s="48"/>
-      <c r="S3" s="50"/>
-      <c r="T3" s="40"/>
-      <c r="U3" s="40"/>
-      <c r="V3" s="42"/>
-      <c r="W3" s="44"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="45"/>
+      <c r="R3" s="53"/>
+      <c r="S3" s="55"/>
+      <c r="T3" s="45"/>
+      <c r="U3" s="45"/>
+      <c r="V3" s="47"/>
+      <c r="W3" s="49"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A4" s="55"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="2">
         <f>18*2</f>
         <v>36</v>
@@ -1250,8 +1257,8 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="21">
+      <c r="O4" s="34"/>
+      <c r="P4" s="19">
         <f t="shared" ref="P4:P6" si="0">SUM(C4:O4)</f>
         <v>67.2</v>
       </c>
@@ -1259,7 +1266,7 @@
         <f>P4*15/1000</f>
         <v>1.008</v>
       </c>
-      <c r="R4" s="19">
+      <c r="R4" s="18">
         <f>'Рассчет трансформатора'!G4</f>
         <v>26.319999999999997</v>
       </c>
@@ -1270,7 +1277,7 @@
         <f>((P4/1000)*0.02)/(S4/1000000)</f>
         <v>0.61090909090909096</v>
       </c>
-      <c r="U4" s="18">
+      <c r="U4" s="17">
         <f>(T4/10000)*1000000</f>
         <v>61.090909090909093</v>
       </c>
@@ -1278,18 +1285,18 @@
         <f>R4-T4/2-15</f>
         <v>11.014545454545452</v>
       </c>
-      <c r="W4" s="17">
+      <c r="W4" s="16">
         <f>(R4-15)*P4/1000</f>
         <v>0.76070399999999982</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A5" s="55"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="2">
         <f>E4+1.3</f>
         <v>37.299999999999997</v>
@@ -1312,8 +1319,8 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="21">
+      <c r="O5" s="34"/>
+      <c r="P5" s="19">
         <f t="shared" si="0"/>
         <v>68.5</v>
       </c>
@@ -1321,7 +1328,7 @@
         <f>P5*15/1000</f>
         <v>1.0275000000000001</v>
       </c>
-      <c r="R5" s="19">
+      <c r="R5" s="18">
         <f>R4</f>
         <v>26.319999999999997</v>
       </c>
@@ -1332,7 +1339,7 @@
         <f>(((P3+P5)/1000)*0.02)/(S5/1000000)</f>
         <v>0.6227272727272728</v>
       </c>
-      <c r="U5" s="18">
+      <c r="U5" s="17">
         <f>(T5/10000)*1000000</f>
         <v>62.272727272727273</v>
       </c>
@@ -1340,35 +1347,35 @@
         <f>R5-T5/2-15</f>
         <v>11.008636363636359</v>
       </c>
-      <c r="W5" s="17">
+      <c r="W5" s="16">
         <f>(R5-15)*P5/1000</f>
         <v>0.77541999999999978</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A6" s="55"/>
-      <c r="B6" s="25" t="s">
+      <c r="A6" s="39"/>
+      <c r="B6" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24">
+      <c r="C6" s="24"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22">
         <f>0.88*2</f>
         <v>1.76</v>
       </c>
-      <c r="J6" s="24">
+      <c r="J6" s="22">
         <v>4.2</v>
       </c>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="23">
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="21">
         <f t="shared" si="0"/>
         <v>5.96</v>
       </c>
@@ -1376,7 +1383,7 @@
         <f>P6*30/1000</f>
         <v>0.17880000000000001</v>
       </c>
-      <c r="R6" s="19">
+      <c r="R6" s="18">
         <f>'Рассчет трансформатора'!G2</f>
         <v>42.48</v>
       </c>
@@ -1387,7 +1394,7 @@
         <f t="shared" ref="T6" si="1">((P6/1000)*0.02)/(S6/1000000)</f>
         <v>0.25361702127659574</v>
       </c>
-      <c r="U6" s="18">
+      <c r="U6" s="17">
         <f t="shared" ref="U6:U7" si="2">(T6/10000)*1000000</f>
         <v>25.361702127659576</v>
       </c>
@@ -1395,36 +1402,36 @@
         <f>R6-T6/2-30</f>
         <v>12.353191489361699</v>
       </c>
-      <c r="W6" s="17">
+      <c r="W6" s="16">
         <f>(R6-30)*P6/1000</f>
         <v>7.4380799999999983E-2</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A7" s="55"/>
-      <c r="B7" s="25" t="s">
+      <c r="A7" s="39"/>
+      <c r="B7" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24">
+      <c r="C7" s="24"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22">
         <f>I6</f>
         <v>1.76</v>
       </c>
-      <c r="J7" s="24">
+      <c r="J7" s="22">
         <f>J6</f>
         <v>4.2</v>
       </c>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="23">
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="21">
         <f t="shared" ref="P7" si="3">SUM(C7:O7)</f>
         <v>5.96</v>
       </c>
@@ -1432,7 +1439,7 @@
         <f>P7*30/1000</f>
         <v>0.17880000000000001</v>
       </c>
-      <c r="R7" s="19">
+      <c r="R7" s="18">
         <f>R6</f>
         <v>42.48</v>
       </c>
@@ -1443,7 +1450,7 @@
         <f t="shared" ref="T7" si="4">((P7/1000)*0.02)/(S7/1000000)</f>
         <v>0.25361702127659574</v>
       </c>
-      <c r="U7" s="18">
+      <c r="U7" s="17">
         <f t="shared" si="2"/>
         <v>25.361702127659576</v>
       </c>
@@ -1451,27 +1458,27 @@
         <f>R7-T7/2-30</f>
         <v>12.353191489361699</v>
       </c>
-      <c r="W7" s="17">
+      <c r="W7" s="16">
         <f>(R7-30)*P7/1000</f>
         <v>7.4380799999999983E-2</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A8" s="55"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="W8" s="6"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A9" s="55"/>
-      <c r="B9" s="51" t="s">
+      <c r="A9" s="39"/>
+      <c r="B9" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
       <c r="G9" s="6">
         <f>SUM(Q2:Q7)</f>
         <v>3.7420999999999998</v>
@@ -1481,14 +1488,14 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="55"/>
-      <c r="B10" s="52" t="s">
+      <c r="A10" s="39"/>
+      <c r="B10" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="6">
         <f>SUM(W2:W7)</f>
         <v>3.015809</v>
@@ -1496,17 +1503,17 @@
       <c r="H10" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="22"/>
+      <c r="K10" s="20"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A11" s="55"/>
-      <c r="B11" s="53" t="s">
+      <c r="A11" s="39"/>
+      <c r="B11" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
       <c r="G11">
         <v>3</v>
       </c>
@@ -1515,14 +1522,14 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A12" s="55"/>
-      <c r="B12" s="52" t="s">
+      <c r="A12" s="39"/>
+      <c r="B12" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
       <c r="G12" s="6">
         <f>230*G11/1000</f>
         <v>0.69</v>
@@ -1531,32 +1538,26 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="55"/>
-      <c r="B13" s="56" t="s">
+    <row r="13" spans="1:23" s="38" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="39"/>
+      <c r="B13" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="57">
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="37">
         <f>G12+G10+G9</f>
         <v>7.4479089999999992</v>
       </c>
-      <c r="H13" s="58" t="s">
+      <c r="H13" s="38" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A1:A13"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
     <mergeCell ref="U2:U3"/>
     <mergeCell ref="V2:V3"/>
     <mergeCell ref="W2:W3"/>
@@ -1565,6 +1566,12 @@
     <mergeCell ref="R2:R3"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="T2:T3"/>
+    <mergeCell ref="A1:A13"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1576,7 +1583,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1591,7 +1598,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="56" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1615,7 +1622,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="54"/>
+      <c r="A2" s="56"/>
       <c r="B2" s="2">
         <v>30</v>
       </c>
@@ -1641,7 +1648,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="54"/>
+      <c r="A3" s="56"/>
       <c r="B3" s="2">
         <f>-B2</f>
         <v>-30</v>
@@ -1669,7 +1676,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="54"/>
+      <c r="A4" s="56"/>
       <c r="B4" s="2">
         <v>20</v>
       </c>
@@ -1695,7 +1702,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="54"/>
+      <c r="A5" s="56"/>
       <c r="B5" s="2">
         <f>-B4</f>
         <v>-20</v>
@@ -1723,7 +1730,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="54"/>
+      <c r="A6" s="56"/>
       <c r="B6" s="2">
         <v>7</v>
       </c>
@@ -1755,7 +1762,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="56" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1774,12 +1781,12 @@
       <c r="G11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="28" t="s">
+      <c r="H11" s="26" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="54"/>
+      <c r="A12" s="56"/>
       <c r="B12" s="2">
         <v>25</v>
       </c>
@@ -1795,7 +1802,7 @@
         <f>(B12*1.41)-1.2</f>
         <v>34.049999999999997</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G12" s="27">
         <v>35.4</v>
       </c>
       <c r="H12" s="2">
@@ -1804,7 +1811,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="54"/>
+      <c r="A13" s="56"/>
       <c r="B13" s="2">
         <f>-B12</f>
         <v>-25</v>
@@ -1822,7 +1829,7 @@
         <f>(B13*1.41)+1.2</f>
         <v>-34.049999999999997</v>
       </c>
-      <c r="G13" s="29">
+      <c r="G13" s="27">
         <v>-35.4</v>
       </c>
       <c r="H13" s="2">
@@ -1831,7 +1838,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="54"/>
+      <c r="A14" s="56"/>
       <c r="B14" s="2">
         <v>15</v>
       </c>
@@ -1847,7 +1854,7 @@
         <f>(B14*1.41)-1.2</f>
         <v>19.95</v>
       </c>
-      <c r="G14" s="29">
+      <c r="G14" s="27">
         <v>19.739999999999998</v>
       </c>
       <c r="H14" s="2">
@@ -1856,7 +1863,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="54"/>
+      <c r="A15" s="56"/>
       <c r="B15" s="2">
         <f>-B14</f>
         <v>-15</v>
@@ -1874,7 +1881,7 @@
         <f>(B15*1.41)+1.2</f>
         <v>-19.95</v>
       </c>
-      <c r="G15" s="29">
+      <c r="G15" s="27">
         <v>-19.739999999999998</v>
       </c>
       <c r="H15" s="2">
@@ -1883,7 +1890,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="54"/>
+      <c r="A16" s="56"/>
       <c r="B16" s="2">
         <v>5</v>
       </c>
@@ -1899,7 +1906,7 @@
         <f>(B16*1.41)-0.6</f>
         <v>6.45</v>
       </c>
-      <c r="G16" s="29">
+      <c r="G16" s="27">
         <f t="shared" ref="G16" si="3">F16*1.1</f>
         <v>7.0950000000000006</v>
       </c>
@@ -1935,86 +1942,86 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="2">
         <f>B3*(1+(B5/B4))+(B2*B5)</f>
         <v>15.006363636363634</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F1" s="2">
         <f>-F3*(1+(F5/F4))+(-F2*F5)</f>
         <v>-15.042363636363635</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="2">
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="F2" s="2">
         <v>6.4999999999999994E-5</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2">
         <v>1.25</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="F3" s="2">
         <f>B3</f>
         <v>1.25</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2">
         <v>220</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" s="2">
         <f>B4</f>
         <v>220</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" s="6">
         <f>(F$19/F4)*F$19</f>
@@ -2026,23 +2033,23 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2">
         <v>2400</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="F5" s="2">
         <f>B5</f>
         <v>2400</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H5" s="6">
         <f>((F$19+F1)/F5)*(F$19+F1)</f>
@@ -2054,86 +2061,86 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" s="2">
         <f>B11*(1+(B13/B12))+(B10*B13)</f>
         <v>29.923333333333336</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F9" s="2">
         <f>-F11*(1+(F13/F12))+(-F10*F13)</f>
         <v>-30.025333333333336</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="2">
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="F10" s="2">
         <v>6.4999999999999994E-5</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="2">
         <v>1.25</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="F11" s="2">
         <f>B11</f>
         <v>1.25</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="2">
         <v>300</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F12" s="2">
         <f>B12</f>
         <v>300</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H12" s="6">
         <f>(F$19/F12)*F$19</f>
@@ -2145,23 +2152,23 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="2">
         <v>6800</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="F13" s="2">
         <f>B13</f>
         <v>6800</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H13" s="6">
         <f>((F$19+F9)/F13)*(F$19+F9)</f>
@@ -2173,86 +2180,86 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="2">
         <f>B19*(1+(B21/B20))+(B18*B21)</f>
         <v>7.5549999999999997</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F17" s="2">
         <f>-F19*(1+(F21/F20))+(-F18*F21)</f>
         <v>-7.5715000000000003</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="2">
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="F18" s="2">
         <v>6.4999999999999994E-5</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="2">
         <v>1.25</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="F19" s="2">
         <f>B19</f>
         <v>1.25</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="2">
         <v>220</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F20" s="2">
         <f>B20</f>
         <v>220</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H20" s="6">
         <f>(F$19/F20)*F$19</f>
@@ -2264,23 +2271,23 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="2">
         <v>1100</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="F21" s="2">
         <f>B21</f>
         <v>1100</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H21" s="6">
         <f>((F$19+F17)/F21)*(F$19+F17)</f>
@@ -2292,7 +2299,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>